<commit_message>
after Laurent. Need to work more...
</commit_message>
<xml_diff>
--- a/src/lithium/data/lithiumMars-juin 2017 NHE1-2.xlsx
+++ b/src/lithium/data/lithiumMars-juin 2017 NHE1-2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32780" windowHeight="18660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1005,22 +1005,22 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
-                <c:pt idx="3" formatCode="0.0">
+                <c:pt idx="3" formatCode="#,#00">
                   <c:v>-8.771987800000001</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.0">
+                <c:pt idx="4" formatCode="#,#00">
                   <c:v>-8.7024606</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.0">
+                <c:pt idx="6" formatCode="#,#00">
                   <c:v>-13.1915437</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="0.0">
+                <c:pt idx="8" formatCode="#,#00">
                   <c:v>-12.9250522</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="0.0">
+                <c:pt idx="10" formatCode="#,#00">
                   <c:v>-12.8275887</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="0.0">
+                <c:pt idx="17" formatCode="#,#00">
                   <c:v>-12.9629817</c:v>
                 </c:pt>
               </c:numCache>
@@ -1170,11 +1170,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2130804824"/>
-        <c:axId val="-2130800856"/>
+        <c:axId val="2048898696"/>
+        <c:axId val="2038243944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2130804824"/>
+        <c:axId val="2048898696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="130.0"/>
@@ -1212,12 +1212,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="-2130800856"/>
+        <c:crossAx val="2038243944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2130800856"/>
+        <c:axId val="2038243944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-6.0"/>
@@ -1254,7 +1254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130804824"/>
+        <c:crossAx val="2048898696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1369,7 +1369,7 @@
             <c:numRef>
               <c:f>Feuil1!$K$37:$K$51</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
                   <c:v>-11.6644118</c:v>
@@ -1505,11 +1505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131336008"/>
-        <c:axId val="-2131341784"/>
+        <c:axId val="2038336280"/>
+        <c:axId val="2038341976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131336008"/>
+        <c:axId val="2038336280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3700.0"/>
@@ -1552,12 +1552,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="-2131341784"/>
+        <c:crossAx val="2038341976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131341784"/>
+        <c:axId val="2038341976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,11 +1589,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131336008"/>
+        <c:crossAx val="2038336280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1661,7 +1661,7 @@
             <c:numRef>
               <c:f>Feuil1!$G$37:$G$47</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.259365994236311</c:v>
@@ -1685,7 +1685,7 @@
             <c:numRef>
               <c:f>Feuil1!$K$37:$K$47</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
                   <c:v>-11.6644118</c:v>
@@ -1806,11 +1806,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131379224"/>
-        <c:axId val="-2131384776"/>
+        <c:axId val="2047949480"/>
+        <c:axId val="2047943704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131379224"/>
+        <c:axId val="2047949480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1847,16 +1847,16 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="-2131384776"/>
+        <c:crossAx val="2047943704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131384776"/>
+        <c:axId val="2047943704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,11 +1888,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131379224"/>
+        <c:crossAx val="2047949480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1975,19 +1975,19 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
-                <c:pt idx="0" formatCode="0.0">
+                <c:pt idx="0" formatCode="#,#00">
                   <c:v>5.072046109510086</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.0">
+                <c:pt idx="3" formatCode="#,#00">
                   <c:v>25.36023054755043</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.0">
+                <c:pt idx="5" formatCode="#,#00">
                   <c:v>23.05475504322767</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="0.0">
+                <c:pt idx="7" formatCode="#,#00">
                   <c:v>23.63112391930836</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0.0">
+                <c:pt idx="14" formatCode="#,#00">
                   <c:v>22.47838616714698</c:v>
                 </c:pt>
               </c:numCache>
@@ -1997,7 +1997,7 @@
             <c:numRef>
               <c:f>Feuil1!$K$20:$K$34</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>-8.771987800000001</c:v>
@@ -2241,11 +2241,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131421224"/>
-        <c:axId val="-2131428616"/>
+        <c:axId val="2047961208"/>
+        <c:axId val="2047974824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131421224"/>
+        <c:axId val="2047961208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2277,16 +2277,16 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="-2131428616"/>
+        <c:crossAx val="2047974824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131428616"/>
+        <c:axId val="2047974824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-8.0"/>
@@ -2324,11 +2324,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131421224"/>
+        <c:crossAx val="2047961208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2834,11 +2834,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131474584"/>
-        <c:axId val="-2131482424"/>
+        <c:axId val="2047884344"/>
+        <c:axId val="2047876776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131474584"/>
+        <c:axId val="2047884344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2865,18 +2865,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131482424"/>
+        <c:crossAx val="2047876776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131482424"/>
+        <c:axId val="2047876776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,7 +2918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131474584"/>
+        <c:crossAx val="2047884344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3193,11 +3194,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131505416"/>
-        <c:axId val="-2131509208"/>
+        <c:axId val="-2116933992"/>
+        <c:axId val="-2116931000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2131505416"/>
+        <c:axId val="-2116933992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3207,12 +3208,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131509208"/>
+        <c:crossAx val="-2116931000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131509208"/>
+        <c:axId val="-2116931000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3222,11 +3223,133 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131505416"/>
+        <c:crossAx val="-2116933992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$O$38:$O$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>229.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>233.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>233.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>485.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>394.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>794.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2181.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2341.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2050139400"/>
+        <c:axId val="2136935928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2050139400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2136935928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2136935928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2050139400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3475,15 +3598,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3497,6 +3620,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Graphique 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4001,8 +4154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B134" sqref="B134:K149"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38:S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>